<commit_message>
correctif mineur mise en forme responsive
</commit_message>
<xml_diff>
--- a/FRONT/plan de Test JS.xlsx
+++ b/FRONT/plan de Test JS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1 - Formation\1 - OPENCLASSROOM\P5 JS FRONT ORINOCO\FRONT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13018E89-5927-4027-8484-BFE433BBF5C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686AED33-5CB0-40DC-B884-9F9C119D220D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{81C23B03-E752-4922-9E38-D23EBFE27495}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="76">
   <si>
     <t>Fichier</t>
   </si>
@@ -192,12 +192,6 @@
     <t>tester différente valeur de chiffre en paramètre, l'absence de valeur</t>
   </si>
   <si>
-    <t xml:space="preserve">un Boolean </t>
-  </si>
-  <si>
-    <t>Un entier égal au nombre de produit commandé</t>
-  </si>
-  <si>
     <t>Un entier égal au montant total du panier</t>
   </si>
   <si>
@@ -211,13 +205,67 @@
   </si>
   <si>
     <t>met a jour l'élément "compteur de produit du dom"</t>
+  </si>
+  <si>
+    <t>ne retourne rien - ne retourne pas un entier (cela casse l'UX)</t>
+  </si>
+  <si>
+    <t>passer en argument un tableau vide, une variable autre qu'un tableau</t>
+  </si>
+  <si>
+    <t>un Boolean égale à true si tout les champs du formulaire sont bien rempli</t>
+  </si>
+  <si>
+    <t>Laisser des champs du formulaire vide - mettre des données invalides</t>
+  </si>
+  <si>
+    <t>passer un argument quelconque</t>
+  </si>
+  <si>
+    <t>Une mise a jour du local storage avec l'ajout de l'objet passé en argument</t>
+  </si>
+  <si>
+    <t>pas d'argument - l'argument n'est pas un objet valide</t>
+  </si>
+  <si>
+    <t>pas de mise à jour du local storage</t>
+  </si>
+  <si>
+    <t>Une mise a jour du local storage avec l'objet passé en argument retiré</t>
+  </si>
+  <si>
+    <t>Un entier égal au nombre de produit dans le panier</t>
+  </si>
+  <si>
+    <t>créer le body de la request envoyé au serveur lors de la commande</t>
+  </si>
+  <si>
+    <t>ne retourne rien - ne retourne pas un objet</t>
+  </si>
+  <si>
+    <t>l'argument n'est pas un objet - l'objet en argument ne contient pas les élément attendu par l'API</t>
+  </si>
+  <si>
+    <t>ne retourne rien - retourne une valeur erronée</t>
+  </si>
+  <si>
+    <t>valider le formulaire sans avoir de produit dans le panier - mettre des info erronée dans le formulaire</t>
+  </si>
+  <si>
+    <t>renvoi un élément du dom avec la confirmation de la commande ou un message d'erreur si un problème  est survenu</t>
+  </si>
+  <si>
+    <t>gère les évènements associé à la soumission du formulaire de commande</t>
+  </si>
+  <si>
+    <t>forcer un argument quelconque</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,8 +281,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,8 +324,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -262,16 +345,118 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,17 +771,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93A3891-9B76-4772-A035-8FA5B193D239}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="28.109375" customWidth="1"/>
-    <col min="4" max="4" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.21875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -609,293 +793,396 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>59</v>
       </c>
+      <c r="F6" s="9" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="E8" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="E10" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="E11" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="E13" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="E14" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D15" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+    </row>
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="E24" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="B25" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E25" s="9" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" t="s">
-        <v>56</v>
-      </c>
+      <c r="F25" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>